<commit_message>
grouped schema of all tables in one file
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/Excel worksheets/factors.xlsx
+++ b/src/main/resources/Data/Excel worksheets/factors.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\darshan\SparkProject\src\main\resources\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\darshan\SparkProject\src\main\resources\Data\Excel worksheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="911" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="106">
   <si>
     <t>customer_id</t>
   </si>
@@ -850,10 +850,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M105"/>
+  <dimension ref="A1:I105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="D74" sqref="D74:E74"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M9" sqref="L6:M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -866,7 +866,7 @@
     <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -895,7 +895,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
@@ -924,7 +924,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>12</v>
       </c>
@@ -953,7 +953,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -982,7 +982,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>12</v>
       </c>
@@ -1035,14 +1035,8 @@
       <c r="I6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="L6" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -1070,14 +1064,8 @@
       <c r="I7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L7" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
@@ -1105,14 +1093,8 @@
       <c r="I8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="L8" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
@@ -1140,14 +1122,8 @@
       <c r="I9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="L9" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>13</v>
       </c>
@@ -1176,7 +1152,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
         <v>13</v>
       </c>
@@ -1205,7 +1181,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
@@ -1234,7 +1210,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>14</v>
       </c>
@@ -1263,7 +1239,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>14</v>
       </c>
@@ -1292,7 +1268,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>14</v>
       </c>
@@ -1321,7 +1297,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
         <v>14</v>
       </c>

</xml_diff>